<commit_message>
Commit. Done Performance Analysis.
</commit_message>
<xml_diff>
--- a/Results/ModelGeneralization/classes_output_openai_gpt-5-mini_OPS.xlsx
+++ b/Results/ModelGeneralization/classes_output_openai_gpt-5-mini_OPS.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\Projects\PythonProject\DMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\Projects\DMP\Results\ModelGeneralization\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE28DD0-D316-4791-BA5E-524ADCF83AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Performance Metrics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -256,7 +268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -610,19 +622,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,13 +642,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -644,43 +656,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -696,13 +708,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -710,25 +722,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -736,7 +748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -744,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -752,7 +764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -760,7 +772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -768,13 +780,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -782,19 +794,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -802,25 +814,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -828,13 +840,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -842,19 +854,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -862,37 +874,37 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -900,67 +912,67 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -968,19 +980,19 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -988,7 +1000,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -996,7 +1008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -1012,13 +1024,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>61</v>
       </c>
@@ -1034,43 +1046,43 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -1084,14 +1096,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1099,7 +1113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1107,7 +1121,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1115,7 +1129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1123,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1131,7 +1145,7 @@
         <v>0.43396226415094341</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>0.6216216216216216</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1147,7 +1161,7 @@
         <v>0.51111111111111118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>

</xml_diff>